<commit_message>
Master data added updated
</commit_message>
<xml_diff>
--- a/MasterData/2. AmortTemplateSYFY.xlsx
+++ b/MasterData/2. AmortTemplateSYFY.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mohammed.saquib\AmortTemplateAutomation\MasterData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mohammed.saquib\eclipse-workspace\amorttemplate\MasterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3897" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="66">
   <si>
     <t>Acquired Movies</t>
   </si>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>Window dates need to be more than or equal to 24 months</t>
-  </si>
-  <si>
-    <t>Pilot 80-20 issue</t>
   </si>
   <si>
     <t>A</t>
@@ -12356,9 +12353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12411,7 +12406,7 @@
         <v>53</v>
       </c>
       <c r="K1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L1" t="s">
         <v>54</v>
@@ -13856,7 +13851,7 @@
         <v>36</v>
       </c>
       <c r="K33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L33" t="s">
         <v>36</v>
@@ -13901,7 +13896,7 @@
         <v>36</v>
       </c>
       <c r="K34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L34" t="s">
         <v>36</v>
@@ -13946,7 +13941,7 @@
         <v>36</v>
       </c>
       <c r="K35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L35" t="s">
         <v>36</v>
@@ -13991,7 +13986,7 @@
         <v>36</v>
       </c>
       <c r="K36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L36" t="s">
         <v>36</v>
@@ -14036,7 +14031,7 @@
         <v>36</v>
       </c>
       <c r="K37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L37" t="s">
         <v>36</v>
@@ -14081,7 +14076,7 @@
         <v>36</v>
       </c>
       <c r="K38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L38" t="s">
         <v>36</v>
@@ -14126,7 +14121,7 @@
         <v>36</v>
       </c>
       <c r="K39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L39" t="s">
         <v>36</v>
@@ -14171,7 +14166,7 @@
         <v>36</v>
       </c>
       <c r="K40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L40" t="s">
         <v>36</v>
@@ -16360,7 +16355,7 @@
         <v>38</v>
       </c>
       <c r="K88" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L88" t="s">
         <v>36</v>
@@ -16405,7 +16400,7 @@
         <v>38</v>
       </c>
       <c r="K89" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L89" t="s">
         <v>36</v>
@@ -16450,7 +16445,7 @@
         <v>38</v>
       </c>
       <c r="K90" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L90" t="s">
         <v>36</v>
@@ -16495,7 +16490,7 @@
         <v>38</v>
       </c>
       <c r="K91" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L91" t="s">
         <v>36</v>
@@ -17122,7 +17117,7 @@
         <v>0</v>
       </c>
       <c r="I105">
-        <v>43.332999999999998</v>
+        <v>43.33</v>
       </c>
       <c r="J105" t="s">
         <v>36</v>
@@ -17138,10 +17133,7 @@
         <v>80Pilot 80-20DocumentaryOriginal Movies</v>
       </c>
       <c r="N105" t="s">
-        <v>61</v>
-      </c>
-      <c r="O105" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
@@ -17170,7 +17162,7 @@
         <v>0</v>
       </c>
       <c r="I106">
-        <v>43.332999999999998</v>
+        <v>43.33</v>
       </c>
       <c r="J106" t="s">
         <v>36</v>
@@ -17186,10 +17178,7 @@
         <v>80Pilot 80-20MoviesOriginal Movies</v>
       </c>
       <c r="N106" t="s">
-        <v>61</v>
-      </c>
-      <c r="O106" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
@@ -17218,7 +17207,7 @@
         <v>0</v>
       </c>
       <c r="I107">
-        <v>43.332999999999998</v>
+        <v>43.33</v>
       </c>
       <c r="J107" t="s">
         <v>36</v>
@@ -17234,10 +17223,7 @@
         <v>80Pilot 80-20OriginalOriginal Movies</v>
       </c>
       <c r="N107" t="s">
-        <v>61</v>
-      </c>
-      <c r="O107" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
@@ -17266,7 +17252,7 @@
         <v>0</v>
       </c>
       <c r="I108">
-        <v>43.332999999999998</v>
+        <v>43.33</v>
       </c>
       <c r="J108" t="s">
         <v>36</v>
@@ -17282,10 +17268,7 @@
         <v>80Pilot 80-20Original MiniSeriesOriginal Movies</v>
       </c>
       <c r="N108" t="s">
-        <v>61</v>
-      </c>
-      <c r="O108" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
@@ -17314,7 +17297,7 @@
         <v>0</v>
       </c>
       <c r="I109">
-        <v>43.332999999999998</v>
+        <v>43.33</v>
       </c>
       <c r="J109" t="s">
         <v>36</v>
@@ -17330,10 +17313,7 @@
         <v>80Pilot 80-20Original SeriesOriginal Movies</v>
       </c>
       <c r="N109" t="s">
-        <v>61</v>
-      </c>
-      <c r="O109" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
@@ -17362,7 +17342,7 @@
         <v>0</v>
       </c>
       <c r="I110">
-        <v>43.332999999999998</v>
+        <v>43.33</v>
       </c>
       <c r="J110" t="s">
         <v>36</v>
@@ -17378,10 +17358,7 @@
         <v>80Pilot 80-20PilotOriginal Movies</v>
       </c>
       <c r="N110" t="s">
-        <v>61</v>
-      </c>
-      <c r="O110" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
@@ -17410,7 +17387,7 @@
         <v>0</v>
       </c>
       <c r="I111">
-        <v>43.332999999999998</v>
+        <v>43.33</v>
       </c>
       <c r="J111" t="s">
         <v>36</v>
@@ -17426,10 +17403,7 @@
         <v>80Pilot 80-20SeriesOriginal Movies</v>
       </c>
       <c r="N111" t="s">
-        <v>61</v>
-      </c>
-      <c r="O111" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
@@ -18682,7 +18656,7 @@
         <v>36</v>
       </c>
       <c r="K138" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L138" t="s">
         <v>36</v>
@@ -18730,7 +18704,7 @@
         <v>36</v>
       </c>
       <c r="K139" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L139" t="s">
         <v>36</v>
@@ -18778,7 +18752,7 @@
         <v>36</v>
       </c>
       <c r="K140" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L140" t="s">
         <v>36</v>
@@ -18826,7 +18800,7 @@
         <v>36</v>
       </c>
       <c r="K141" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L141" t="s">
         <v>36</v>
@@ -18874,7 +18848,7 @@
         <v>36</v>
       </c>
       <c r="K142" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L142" t="s">
         <v>36</v>
@@ -18922,7 +18896,7 @@
         <v>36</v>
       </c>
       <c r="K143" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L143" t="s">
         <v>36</v>
@@ -18970,7 +18944,7 @@
         <v>36</v>
       </c>
       <c r="K144" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L144" t="s">
         <v>36</v>
@@ -19018,7 +18992,7 @@
         <v>36</v>
       </c>
       <c r="K145" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L145" t="s">
         <v>36</v>
@@ -19066,7 +19040,7 @@
         <v>36</v>
       </c>
       <c r="K146" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L146" t="s">
         <v>36</v>
@@ -19114,7 +19088,7 @@
         <v>36</v>
       </c>
       <c r="K147" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L147" t="s">
         <v>36</v>
@@ -19162,7 +19136,7 @@
         <v>36</v>
       </c>
       <c r="K148" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L148" t="s">
         <v>36</v>
@@ -20133,7 +20107,7 @@
         <v>36</v>
       </c>
       <c r="K169" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L169" t="s">
         <v>36</v>
@@ -20226,7 +20200,7 @@
         <v>36</v>
       </c>
       <c r="K171" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L171" t="s">
         <v>36</v>
@@ -20271,7 +20245,7 @@
         <v>36</v>
       </c>
       <c r="K172" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L172" t="s">
         <v>36</v>
@@ -20316,7 +20290,7 @@
         <v>36</v>
       </c>
       <c r="K173" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L173" t="s">
         <v>36</v>
@@ -20361,7 +20335,7 @@
         <v>36</v>
       </c>
       <c r="K174" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L174" t="s">
         <v>36</v>
@@ -20406,7 +20380,7 @@
         <v>36</v>
       </c>
       <c r="K175" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L175" t="s">
         <v>36</v>
@@ -20451,7 +20425,7 @@
         <v>36</v>
       </c>
       <c r="K176" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L176" t="s">
         <v>36</v>

</xml_diff>